<commit_message>
Add Goals and Programmes.
</commit_message>
<xml_diff>
--- a/Uganda/Ordering.xlsx
+++ b/Uganda/Ordering.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github.com\open-word\Q\Uganda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C260CAD-F857-4B51-9DC3-37AD50BC5203}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F262226-72AE-4451-98C2-6BC3929A6C91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{C776B387-F4FE-4EBD-85A1-E8F3FE28FBCF}"/>
+    <workbookView xWindow="3135" yWindow="1905" windowWidth="21600" windowHeight="11835" xr2:uid="{C776B387-F4FE-4EBD-85A1-E8F3FE28FBCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -612,6 +612,71 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>428624</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>57149</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>161926</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Rectangle 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA3AFE92-A350-581A-F71D-EB2F128954AA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6524624" y="16668750"/>
+          <a:ext cx="2676525" cy="1209676"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="57150"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>Goal</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -916,8 +981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5253E909-B6E2-4B3D-9366-925166517572}">
   <dimension ref="B2:B91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="F97" sqref="F97"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>